<commit_message>
added sharing, tweaks, and example randomization
</commit_message>
<xml_diff>
--- a/content.xlsx
+++ b/content.xlsx
@@ -4,7 +4,6 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="IW core skills" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Other wordings" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="134">
   <si>
     <t xml:space="preserve">
 </t>
@@ -335,10 +334,7 @@
   </si>
   <si>
     <t>• Try out leading meetings
-• Lead on smaller things
-• Emily and Matt T and Georgia leading on d&amp;i
-• Gohar on end of months
-• Rebecca, Rowan, John J etc</t>
+• Lead on smaller things</t>
   </si>
   <si>
     <t>• Don't fixate on failure, accept defeat and focus on the future</t>
@@ -641,69 +637,12 @@
     <t>• Works across multiple regions
 • Plays a key role in supporting and challenging leaders throughout the company</t>
   </si>
-  <si>
-    <t>Things we value Framework v1.0</t>
-  </si>
-  <si>
-    <t>Infinite capability Framework v1.0</t>
-  </si>
-  <si>
-    <t>How to be an Infinite</t>
-  </si>
-  <si>
-    <t>Be a great colleague</t>
-  </si>
-  <si>
-    <t>Don't be a dick</t>
-  </si>
-  <si>
-    <t>We figure stuff out</t>
-  </si>
-  <si>
-    <t>Solve things other people can't</t>
-  </si>
-  <si>
-    <t>Don't be afraid to figure stuff out</t>
-  </si>
-  <si>
-    <t>Delivery first</t>
-  </si>
-  <si>
-    <t>Enjoy the challenge</t>
-  </si>
-  <si>
-    <t>Leaderful practice</t>
-  </si>
-  <si>
-    <t>Empower yourself and others</t>
-  </si>
-  <si>
-    <t>Know the business</t>
-  </si>
-  <si>
-    <t>Grow the business</t>
-  </si>
-  <si>
-    <t>Be resourceful</t>
-  </si>
-  <si>
-    <t>Embrace failure and ambiguity</t>
-  </si>
-  <si>
-    <t>Experiment and evolve</t>
-  </si>
-  <si>
-    <t>See change as opportunity</t>
-  </si>
-  <si>
-    <t>Be comfortable with failure and ambiguity</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -775,10 +714,6 @@
       <b/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -840,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -925,9 +860,6 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -945,10 +877,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -9496,16 +9424,16 @@
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="B23:B30"/>
+    <mergeCell ref="B15:B22"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="I5:I46"/>
     <mergeCell ref="B31:B38"/>
-    <mergeCell ref="C3:I3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="B39:B46"/>
     <mergeCell ref="A7:A46"/>
-    <mergeCell ref="B15:B22"/>
     <mergeCell ref="B7:B14"/>
-    <mergeCell ref="I5:I46"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -9513,96 +9441,4 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="28.0"/>
-    <col customWidth="1" min="3" max="3" width="28.71"/>
-    <col customWidth="1" min="4" max="4" width="18.14"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>